<commit_message>
dag with decorator added
</commit_message>
<xml_diff>
--- a/data/raw/tatasteel.xlsx
+++ b/data/raw/tatasteel.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G247"/>
+  <dimension ref="A1:G248"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6624,6 +6624,31 @@
         <v>62282856</v>
       </c>
     </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>TATASTEEL.NS</t>
+        </is>
+      </c>
+      <c r="B248" s="2" t="n">
+        <v>45768</v>
+      </c>
+      <c r="C248" t="n">
+        <v>137.6499938965</v>
+      </c>
+      <c r="D248" t="n">
+        <v>140.3000030518</v>
+      </c>
+      <c r="E248" t="n">
+        <v>137.0500030518</v>
+      </c>
+      <c r="F248" t="n">
+        <v>139.1799926758</v>
+      </c>
+      <c r="G248" t="n">
+        <v>26503486</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>